<commit_message>
Fixed critical bug in f function
Loop in function changed protein producing parameters but didnt perform the FBA after changing parameters
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/parameters.xlsx
+++ b/iGEM simulation environment/Scripts/parameters.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{11C2AAE7-A30A-4443-9891-09464F3CCEB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3552DB64-1370-488C-B3D3-CA4261F505C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9810" windowHeight="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$135</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="173">
   <si>
     <t>%Glucose uptake kinetic parameters</t>
   </si>
@@ -530,6 +530,18 @@
   </si>
   <si>
     <t>mmol/L</t>
+  </si>
+  <si>
+    <t>mM/L</t>
+  </si>
+  <si>
+    <t>vmax_c4</t>
+  </si>
+  <si>
+    <t>ks_c4</t>
+  </si>
+  <si>
+    <t>%Carbon dioxide uptake kinetic parameters</t>
   </si>
 </sst>
 </file>
@@ -863,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,6 +995,7 @@
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1146,14 +1159,11 @@
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
-        <v>1</v>
+      <c r="B29" s="1">
+        <v>0.623</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0.623</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,226 +1611,229 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>90</v>
+      <c r="A75" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="B75" s="2">
-        <v>0</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>89</v>
+        <v>2.5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>91</v>
+      <c r="A76" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B76" s="2">
-        <v>5.5</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B77" s="2">
-        <v>10.9</v>
+        <v>0</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B78" s="2">
-        <v>0.3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B79" s="2">
-        <v>1</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B80" s="2">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B81" s="2">
-        <v>0</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B82" s="2">
-        <v>150</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B83" s="2">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B84" s="2">
-        <v>4.32</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B85" s="2">
-        <v>21.065000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="B86" s="2">
-        <v>20</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B87" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>103</v>
+        <v>21.065000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B88" s="2">
-        <v>1.4079999999999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B89" s="2">
-        <v>3.4910000000000001</v>
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B90" s="2">
-        <v>2.2120000000000002</v>
+        <v>1.4079999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B91" s="2">
-        <v>3.4609999999999999</v>
+        <v>3.4910000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B92" s="2">
-        <v>2.7629999999999999</v>
+        <v>2.2120000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B93" s="2">
-        <v>0.47199999999999998</v>
+        <v>3.4609999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B94" s="2">
-        <v>1.2589999999999999</v>
+        <v>2.7629999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B95" s="2">
-        <v>5.0979999999999999</v>
+        <v>0.47199999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" s="2">
-        <v>2.734</v>
+        <v>1.2589999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B97" s="2">
-        <v>0</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>114</v>
+        <v>5.0979999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B98" s="2">
-        <v>0</v>
+        <v>2.734</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B99" s="2">
         <v>0</v>
       </c>
+      <c r="C99" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B100" s="2">
         <v>0</v>
@@ -1828,7 +1841,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B101" s="2">
         <v>0</v>
@@ -1836,7 +1849,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B102" s="2">
         <v>0</v>
@@ -1844,7 +1857,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B103" s="2">
         <v>0</v>
@@ -1852,49 +1865,49 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B104" s="2">
-        <v>1</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D104" s="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B105" s="2">
         <v>0</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B106" s="2">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D106" s="2"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B107" s="2">
         <v>0</v>
       </c>
+      <c r="C107" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B108" s="2">
         <v>0</v>
@@ -1902,7 +1915,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B109" s="2">
         <v>0</v>
@@ -1910,45 +1923,45 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B110" s="2">
-        <v>100</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B111" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B112" s="2">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B113" s="2">
-        <v>250</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B114" s="2">
         <v>500</v>
@@ -1956,135 +1969,135 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B115" s="2">
-        <v>1</v>
+        <v>500</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B116" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>103</v>
+        <v>500</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B117" s="2">
-        <v>1.4079999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B118" s="2">
-        <v>3.4910000000000001</v>
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B119" s="2">
-        <v>2.2120000000000002</v>
+        <v>1.4079999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B120" s="2">
-        <v>3.4609999999999999</v>
+        <v>3.4910000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B121" s="2">
-        <v>2.7629999999999999</v>
+        <v>2.2120000000000002</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B122" s="2">
-        <f>D122*10</f>
-        <v>4.72</v>
-      </c>
-      <c r="D122" s="2">
-        <v>0.47199999999999998</v>
+        <v>3.4609999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B123" s="2">
-        <v>1.2589999999999999</v>
+        <v>2.7629999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B124" s="2">
-        <v>5.0979999999999999</v>
+        <f>D124*10</f>
+        <v>4.72</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0.47199999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B125" s="2">
-        <v>2.734</v>
+        <v>1.2589999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B126" s="2">
-        <v>0</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>103</v>
+        <v>5.0979999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B127" s="2">
-        <v>0</v>
+        <v>2.734</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B128" s="2">
         <v>0</v>
       </c>
+      <c r="C128" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B129" s="2">
         <v>0</v>
@@ -2092,15 +2105,15 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B130" s="2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B131" s="2">
         <v>0</v>
@@ -2108,65 +2121,81 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B132" s="2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="B133" s="2">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D133" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B134" s="2">
-        <v>10</v>
-      </c>
-      <c r="C134" t="s">
-        <v>161</v>
-      </c>
-      <c r="D134" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="B135" s="2">
-        <v>60</v>
-      </c>
-      <c r="C135" t="s">
-        <v>164</v>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="D135" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B136" s="2">
+        <v>10</v>
+      </c>
+      <c r="C136" t="s">
+        <v>161</v>
+      </c>
+      <c r="D136" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B137" s="2">
+        <v>60</v>
+      </c>
+      <c r="C137" t="s">
+        <v>164</v>
+      </c>
+      <c r="D137" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B136">
+      <c r="B138">
         <v>0.01</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C138" t="s">
         <v>167</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D138" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added extra loop to reduce protein production if Sbo model is not solvable
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/parameters.xlsx
+++ b/iGEM simulation environment/Scripts/parameters.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3552DB64-1370-488C-B3D3-CA4261F505C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9D366E4E-0F81-49D0-9BEE-3A29E401E500}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9810" windowHeight="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1688,7 @@
         <v>97</v>
       </c>
       <c r="B83" s="2">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>96</v>
@@ -1731,7 +1731,7 @@
         <v>130</v>
       </c>
       <c r="B88" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>131</v>
       </c>
       <c r="B106" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>165</v>
@@ -1988,7 +1988,7 @@
         <v>159</v>
       </c>
       <c r="B117" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>156</v>
       </c>
       <c r="B132" s="2">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>160</v>
       </c>
       <c r="B136" s="2">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="C136" t="s">
         <v>161</v>
@@ -2190,7 +2190,7 @@
         <v>166</v>
       </c>
       <c r="B138">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C138" t="s">
         <v>167</v>

</xml_diff>